<commit_message>
updated cnn thaitale results.
</commit_message>
<xml_diff>
--- a/output/DEEP_TT.xlsx
+++ b/output/DEEP_TT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pree\Thai_SA_journal\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CAD8BBB-2F76-424B-ABDE-83600ECFA48F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9E82C1C-ADEC-4AEF-A195-AF9A64524D25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3900" yWindow="1740" windowWidth="15225" windowHeight="13605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RESULT" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="156">
   <si>
     <t>0RF</t>
   </si>
@@ -464,34 +464,43 @@
     <t>BERT</t>
   </si>
   <si>
-    <t>0.6645±0.0058</t>
-  </si>
-  <si>
-    <t>0.6125±0.0296</t>
-  </si>
-  <si>
-    <t>0.4446±0.0167</t>
-  </si>
-  <si>
-    <t>0.4041±0.0119</t>
-  </si>
-  <si>
-    <t>0.808±0.0043</t>
-  </si>
-  <si>
-    <t>0.5149±0.0154</t>
-  </si>
-  <si>
-    <t>0.6712±0.0062</t>
-  </si>
-  <si>
-    <t>0.4177±0.013</t>
-  </si>
-  <si>
-    <t>0.5189±0.0205</t>
-  </si>
-  <si>
     <t>Bi-LSTM</t>
+  </si>
+  <si>
+    <t>0.5483±0.0171</t>
+  </si>
+  <si>
+    <t>0.51±0.0269</t>
+  </si>
+  <si>
+    <t>0.4728±0.033</t>
+  </si>
+  <si>
+    <t>0.2519±0.0381</t>
+  </si>
+  <si>
+    <t>0.6503±0.0332</t>
+  </si>
+  <si>
+    <t>0.4904±0.0282</t>
+  </si>
+  <si>
+    <t>0.5±0.0312</t>
+  </si>
+  <si>
+    <t>0.4836±0.0659</t>
+  </si>
+  <si>
+    <t>0.4437±0.0421</t>
+  </si>
+  <si>
+    <t>0.1876±0.0514</t>
+  </si>
+  <si>
+    <t>0.634±0.0239</t>
+  </si>
+  <si>
+    <t>0.4591±0.0274</t>
   </si>
 </sst>
 </file>
@@ -1371,8 +1380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D5C4ABC-024F-46B2-BF47-2362A367FE2E}">
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1431,45 +1440,45 @@
         <v>141</v>
       </c>
       <c r="B3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="I3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="J3" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="K3" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="L3" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="M3" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="N3" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:14">

</xml_diff>